<commit_message>
Graph corrections & OS optimisations
</commit_message>
<xml_diff>
--- a/REB.xlsx
+++ b/REB.xlsx
@@ -1,13 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -521,7 +521,7 @@
         <v>292.160105375089</v>
       </c>
       <c r="G2" t="n">
-        <v>23498833.19469264</v>
+        <v>23498833.19469265</v>
       </c>
       <c r="H2" t="n">
         <v>153342</v>
@@ -530,13 +530,13 @@
         <v>0.7817333333333334</v>
       </c>
       <c r="J2" t="n">
-        <v>153.2445983141777</v>
+        <v>153.2445983141778</v>
       </c>
       <c r="K2" t="n">
         <v>5.224542126175285</v>
       </c>
       <c r="L2" t="n">
-        <v>29.33168010004411</v>
+        <v>29.33168010004412</v>
       </c>
       <c r="M2" t="n">
         <v>55.92071004870427</v>
@@ -615,7 +615,7 @@
         <v>251.7003107406596</v>
       </c>
       <c r="G4" t="n">
-        <v>85398933.9244322</v>
+        <v>85398933.92443219</v>
       </c>
       <c r="H4" t="n">
         <v>633260</v>
@@ -624,7 +624,7 @@
         <v>0.7625666666666667</v>
       </c>
       <c r="J4" t="n">
-        <v>134.8560368954809</v>
+        <v>134.8560368954808</v>
       </c>
       <c r="K4" t="n">
         <v>5.202284946236559</v>
@@ -668,7 +668,7 @@
         <v>148241</v>
       </c>
       <c r="I5" t="n">
-        <v>0.7723916666666667</v>
+        <v>0.7723916666666666</v>
       </c>
       <c r="J5" t="n">
         <v>70.40120691607551</v>
@@ -721,13 +721,13 @@
         <v>86.2600938461098</v>
       </c>
       <c r="K6" t="n">
-        <v>5.670888628498196</v>
+        <v>5.670888628498197</v>
       </c>
       <c r="L6" t="n">
         <v>15.21103648776008</v>
       </c>
       <c r="M6" t="n">
-        <v>32.77722740410934</v>
+        <v>32.77722740410933</v>
       </c>
     </row>
     <row r="7">
@@ -756,7 +756,7 @@
         <v>34.49961582088046</v>
       </c>
       <c r="G7" t="n">
-        <v>4455092.247113372</v>
+        <v>4455092.247113373</v>
       </c>
       <c r="H7" t="n">
         <v>179960</v>
@@ -771,7 +771,7 @@
         <v>5.5</v>
       </c>
       <c r="L7" t="n">
-        <v>4.501093421885037</v>
+        <v>4.501093421885038</v>
       </c>
       <c r="M7" t="n">
         <v>6.272657421978266</v>
@@ -812,16 +812,16 @@
         <v>0.5416583333333334</v>
       </c>
       <c r="J8" t="n">
-        <v>78.99674527894821</v>
+        <v>78.9967452789482</v>
       </c>
       <c r="K8" t="n">
-        <v>6.455869175627239</v>
+        <v>6.45586917562724</v>
       </c>
       <c r="L8" t="n">
-        <v>12.23642287814376</v>
+        <v>12.23642287814375</v>
       </c>
       <c r="M8" t="n">
-        <v>26.77349116618522</v>
+        <v>26.77349116618521</v>
       </c>
     </row>
     <row r="9">
@@ -862,13 +862,13 @@
         <v>75.62983199488137</v>
       </c>
       <c r="K9" t="n">
-        <v>6.416666666666666</v>
+        <v>6.416666666666667</v>
       </c>
       <c r="L9" t="n">
         <v>11.78646732387762</v>
       </c>
       <c r="M9" t="n">
-        <v>23.32038298895912</v>
+        <v>23.32038298895911</v>
       </c>
     </row>
     <row r="10">
@@ -891,7 +891,7 @@
         </is>
       </c>
       <c r="E10" t="n">
-        <v>82729.41999999998</v>
+        <v>82729.42</v>
       </c>
       <c r="F10" t="n">
         <v>201.7128065740409</v>
@@ -938,10 +938,10 @@
         </is>
       </c>
       <c r="E11" t="n">
-        <v>49973.24999999999</v>
+        <v>49973.25</v>
       </c>
       <c r="F11" t="n">
-        <v>284.1093857006328</v>
+        <v>284.1093857006329</v>
       </c>
       <c r="G11" t="n">
         <v>14101910.59552569</v>
@@ -962,7 +962,7 @@
         <v>29.85121987849725</v>
       </c>
       <c r="M11" t="n">
-        <v>44.2215818326107</v>
+        <v>44.22158183261071</v>
       </c>
     </row>
     <row r="12">
@@ -988,10 +988,10 @@
         <v>264293.59</v>
       </c>
       <c r="F12" t="n">
-        <v>390.9650242048281</v>
+        <v>390.965024204828</v>
       </c>
       <c r="G12" t="n">
-        <v>108305344.7054132</v>
+        <v>108305344.7054131</v>
       </c>
       <c r="H12" t="n">
         <v>459141</v>
@@ -1000,16 +1000,16 @@
         <v>0.8520083333333334</v>
       </c>
       <c r="J12" t="n">
-        <v>235.8868946694222</v>
+        <v>235.8868946694221</v>
       </c>
       <c r="K12" t="n">
-        <v>6.488429744387457</v>
+        <v>6.488429744387459</v>
       </c>
       <c r="L12" t="n">
-        <v>36.35500482585423</v>
+        <v>36.35500482585422</v>
       </c>
       <c r="M12" t="n">
-        <v>60.25572281845479</v>
+        <v>60.25572281845476</v>
       </c>
     </row>
     <row r="13">
@@ -1044,16 +1044,16 @@
         <v>161040</v>
       </c>
       <c r="I13" t="n">
-        <v>0.7091083333333335</v>
+        <v>0.7091083333333333</v>
       </c>
       <c r="J13" t="n">
         <v>141.865871538429</v>
       </c>
       <c r="K13" t="n">
-        <v>6.588721006880074</v>
+        <v>6.588721006880072</v>
       </c>
       <c r="L13" t="n">
-        <v>21.53162524111885</v>
+        <v>21.53162524111886</v>
       </c>
       <c r="M13" t="n">
         <v>35.6473641788951</v>
@@ -1085,7 +1085,7 @@
         <v>258.8574364344258</v>
       </c>
       <c r="G14" t="n">
-        <v>24098261.38468844</v>
+        <v>24098261.38468845</v>
       </c>
       <c r="H14" t="n">
         <v>176880</v>
@@ -1103,7 +1103,7 @@
         <v>21.67558777050552</v>
       </c>
       <c r="M14" t="n">
-        <v>41.18362281342673</v>
+        <v>41.18362281342674</v>
       </c>
     </row>
     <row r="15">
@@ -1138,16 +1138,16 @@
         <v>160600</v>
       </c>
       <c r="I15" t="n">
-        <v>0.9248749999999998</v>
+        <v>0.924875</v>
       </c>
       <c r="J15" t="n">
         <v>199.064661833696</v>
       </c>
       <c r="K15" t="n">
-        <v>7.086917562724016</v>
+        <v>7.086917562724015</v>
       </c>
       <c r="L15" t="n">
-        <v>28.08903307705205</v>
+        <v>28.08903307705206</v>
       </c>
       <c r="M15" t="n">
         <v>35.4372884841056</v>
@@ -1173,7 +1173,7 @@
         </is>
       </c>
       <c r="E16" t="n">
-        <v>47324.48000000001</v>
+        <v>47324.48</v>
       </c>
       <c r="F16" t="n">
         <v>448.386587461132</v>
@@ -1185,13 +1185,13 @@
         <v>153300</v>
       </c>
       <c r="I16" t="n">
-        <v>0.6016833333333335</v>
+        <v>0.6016833333333333</v>
       </c>
       <c r="J16" t="n">
         <v>153.623079552488</v>
       </c>
       <c r="K16" t="n">
-        <v>6.928708580206275</v>
+        <v>6.928708580206276</v>
       </c>
       <c r="L16" t="n">
         <v>22.17196433854265</v>
@@ -1226,7 +1226,7 @@
         <v>408.0426073309466</v>
       </c>
       <c r="G17" t="n">
-        <v>27646557.30436869</v>
+        <v>27646557.3043687</v>
       </c>
       <c r="H17" t="n">
         <v>149634</v>
@@ -1244,7 +1244,7 @@
         <v>26.88415438802744</v>
       </c>
       <c r="M17" t="n">
-        <v>59.37329098664338</v>
+        <v>59.37329098664337</v>
       </c>
     </row>
     <row r="18">
@@ -1314,7 +1314,7 @@
         </is>
       </c>
       <c r="E19" t="n">
-        <v>52529.88000000001</v>
+        <v>52529.88</v>
       </c>
       <c r="F19" t="n">
         <v>502.8746547995295</v>
@@ -1326,19 +1326,19 @@
         <v>153300</v>
       </c>
       <c r="I19" t="n">
-        <v>0.8759999999999999</v>
+        <v>0.876</v>
       </c>
       <c r="J19" t="n">
         <v>213.0842994990038</v>
       </c>
       <c r="K19" t="n">
-        <v>7.023745519713263</v>
+        <v>7.023745519713262</v>
       </c>
       <c r="L19" t="n">
         <v>30.33770214210477</v>
       </c>
       <c r="M19" t="n">
-        <v>71.59636598281237</v>
+        <v>71.59636598281239</v>
       </c>
     </row>
     <row r="20">
@@ -1455,7 +1455,7 @@
         </is>
       </c>
       <c r="E22" t="n">
-        <v>320138.9399999999</v>
+        <v>320138.94</v>
       </c>
       <c r="F22" t="n">
         <v>377.9998067401887</v>
@@ -1473,13 +1473,13 @@
         <v>160.022653844114</v>
       </c>
       <c r="K22" t="n">
-        <v>7.416666666666668</v>
+        <v>7.416666666666667</v>
       </c>
       <c r="L22" t="n">
         <v>21.57608815875694</v>
       </c>
       <c r="M22" t="n">
-        <v>50.96626607732881</v>
+        <v>50.9662660773288</v>
       </c>
     </row>
     <row r="23">
@@ -1505,16 +1505,16 @@
         <v>40838.15</v>
       </c>
       <c r="F23" t="n">
-        <v>317.1467994672981</v>
+        <v>317.146799467298</v>
       </c>
       <c r="G23" t="n">
-        <v>22800273.3173044</v>
+        <v>22800273.31730439</v>
       </c>
       <c r="H23" t="n">
         <v>204992</v>
       </c>
       <c r="I23" t="n">
-        <v>0.541625</v>
+        <v>0.5416249999999999</v>
       </c>
       <c r="J23" t="n">
         <v>111.2251859453266</v>
@@ -1523,7 +1523,7 @@
         <v>7.273521505376344</v>
       </c>
       <c r="L23" t="n">
-        <v>15.29179309679812</v>
+        <v>15.29179309679811</v>
       </c>
       <c r="M23" t="n">
         <v>43.60292318279031</v>
@@ -1567,7 +1567,7 @@
         <v>157.2100209897406</v>
       </c>
       <c r="K24" t="n">
-        <v>7.333333333333332</v>
+        <v>7.333333333333333</v>
       </c>
       <c r="L24" t="n">
         <v>21.43773013496463</v>
@@ -1599,19 +1599,19 @@
         <v>145830.13</v>
       </c>
       <c r="F25" t="n">
-        <v>404.2435043783971</v>
+        <v>404.2435043783969</v>
       </c>
       <c r="G25" t="n">
-        <v>90849205.98219678</v>
+        <v>90849205.98219676</v>
       </c>
       <c r="H25" t="n">
         <v>453692</v>
       </c>
       <c r="I25" t="n">
-        <v>0.8358416666666666</v>
+        <v>0.8358416666666667</v>
       </c>
       <c r="J25" t="n">
-        <v>200.2442317303298</v>
+        <v>200.2442317303297</v>
       </c>
       <c r="K25" t="n">
         <v>7.381209519484064</v>
@@ -1620,7 +1620,7 @@
         <v>27.12891853316833</v>
       </c>
       <c r="M25" t="n">
-        <v>54.76656682232387</v>
+        <v>54.76656682232386</v>
       </c>
     </row>
     <row r="26">
@@ -1667,7 +1667,7 @@
         <v>27.81955135602923</v>
       </c>
       <c r="M26" t="n">
-        <v>48.35180886713325</v>
+        <v>48.35180886713326</v>
       </c>
     </row>
     <row r="27">
@@ -1690,10 +1690,10 @@
         </is>
       </c>
       <c r="E27" t="n">
-        <v>160789.0699999999</v>
+        <v>160789.07</v>
       </c>
       <c r="F27" t="n">
-        <v>482.0453417031386</v>
+        <v>482.0453417031387</v>
       </c>
       <c r="G27" t="n">
         <v>114165313.2529743</v>
@@ -1708,13 +1708,13 @@
         <v>242.5993498677715</v>
       </c>
       <c r="K27" t="n">
-        <v>7.850933734691808</v>
+        <v>7.850933734691807</v>
       </c>
       <c r="L27" t="n">
         <v>30.90070023082355</v>
       </c>
       <c r="M27" t="n">
-        <v>61.39974657703075</v>
+        <v>61.39974657703078</v>
       </c>
     </row>
     <row r="28">
@@ -1796,19 +1796,19 @@
         <v>1224940</v>
       </c>
       <c r="I29" t="n">
-        <v>0.7956499999999999</v>
+        <v>0.7956500000000001</v>
       </c>
       <c r="J29" t="n">
         <v>160.5945676573344</v>
       </c>
       <c r="K29" t="n">
-        <v>7.769698708073975</v>
+        <v>7.769698708073977</v>
       </c>
       <c r="L29" t="n">
         <v>20.66934300688527</v>
       </c>
       <c r="M29" t="n">
-        <v>51.99767856659194</v>
+        <v>51.99767856659193</v>
       </c>
     </row>
     <row r="30">
@@ -1834,7 +1834,7 @@
         <v>166182.76</v>
       </c>
       <c r="F30" t="n">
-        <v>238.5965003869411</v>
+        <v>238.596500386941</v>
       </c>
       <c r="G30" t="n">
         <v>42607340.67733214</v>
@@ -1843,19 +1843,19 @@
         <v>322439</v>
       </c>
       <c r="I30" t="n">
-        <v>0.8448249999999998</v>
+        <v>0.844825</v>
       </c>
       <c r="J30" t="n">
         <v>132.1407791158394</v>
       </c>
       <c r="K30" t="n">
-        <v>8.337409085675553</v>
+        <v>8.337409085675555</v>
       </c>
       <c r="L30" t="n">
-        <v>15.84914183266713</v>
+        <v>15.84914183266712</v>
       </c>
       <c r="M30" t="n">
-        <v>28.61758346449284</v>
+        <v>28.61758346449283</v>
       </c>
     </row>
     <row r="31">
@@ -1890,7 +1890,7 @@
         <v>213400</v>
       </c>
       <c r="I31" t="n">
-        <v>0.7373750000000001</v>
+        <v>0.737375</v>
       </c>
       <c r="J31" t="n">
         <v>85.73167377083593</v>
@@ -1931,25 +1931,25 @@
         <v>368.4760040924052</v>
       </c>
       <c r="G32" t="n">
-        <v>54186850.22538487</v>
+        <v>54186850.22538488</v>
       </c>
       <c r="H32" t="n">
         <v>356610</v>
       </c>
       <c r="I32" t="n">
-        <v>0.5677249999999999</v>
+        <v>0.567725</v>
       </c>
       <c r="J32" t="n">
-        <v>151.9498898667588</v>
+        <v>151.9498898667589</v>
       </c>
       <c r="K32" t="n">
-        <v>8.629232279859183</v>
+        <v>8.629232279859185</v>
       </c>
       <c r="L32" t="n">
         <v>17.60873794316711</v>
       </c>
       <c r="M32" t="n">
-        <v>42.70090225203883</v>
+        <v>42.70090225203882</v>
       </c>
     </row>
     <row r="33">
@@ -1984,7 +1984,7 @@
         <v>104751.4137931034</v>
       </c>
       <c r="I33" t="n">
-        <v>0.4490166666666666</v>
+        <v>0.4490166666666667</v>
       </c>
       <c r="J33" t="n">
         <v>70.24502091756297</v>
@@ -1996,7 +1996,7 @@
         <v>7.422233374345259</v>
       </c>
       <c r="M33" t="n">
-        <v>28.45397690606227</v>
+        <v>28.45397690606228</v>
       </c>
     </row>
     <row r="34">
@@ -2022,7 +2022,7 @@
         <v>70956.97</v>
       </c>
       <c r="F34" t="n">
-        <v>72.60765771203943</v>
+        <v>72.60765771203944</v>
       </c>
       <c r="G34" t="n">
         <v>4816659.20337001</v>
@@ -2037,10 +2037,10 @@
         <v>55.00981273835095</v>
       </c>
       <c r="K34" t="n">
-        <v>9.689603174603173</v>
+        <v>9.689603174603175</v>
       </c>
       <c r="L34" t="n">
-        <v>5.677199751846785</v>
+        <v>5.677199751846784</v>
       </c>
       <c r="M34" t="n">
         <v>7.493357199843532</v>
@@ -2078,7 +2078,7 @@
         <v>72240</v>
       </c>
       <c r="I35" t="n">
-        <v>0.5448749999999999</v>
+        <v>0.544875</v>
       </c>
       <c r="J35" t="n">
         <v>120.7307355286764</v>
@@ -2113,10 +2113,10 @@
         </is>
       </c>
       <c r="E36" t="n">
-        <v>44111.29999999999</v>
+        <v>44111.3</v>
       </c>
       <c r="F36" t="n">
-        <v>235.438223545687</v>
+        <v>235.4382235456869</v>
       </c>
       <c r="G36" t="n">
         <v>10623009.60635437</v>
@@ -2137,7 +2137,7 @@
         <v>19.53658401922874</v>
       </c>
       <c r="M36" t="n">
-        <v>24.57132563441018</v>
+        <v>24.57132563441017</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Ancillary shaved 14 secs
</commit_message>
<xml_diff>
--- a/REB.xlsx
+++ b/REB.xlsx
@@ -518,10 +518,10 @@
         <v>67417.90000000001</v>
       </c>
       <c r="F2" t="n">
-        <v>292.160105375089</v>
+        <v>296.5995795127912</v>
       </c>
       <c r="G2" t="n">
-        <v>23498833.19469265</v>
+        <v>23853195.83998579</v>
       </c>
       <c r="H2" t="n">
         <v>153342</v>
@@ -530,16 +530,16 @@
         <v>0.7817333333333334</v>
       </c>
       <c r="J2" t="n">
-        <v>153.2445983141778</v>
+        <v>155.5555284265615</v>
       </c>
       <c r="K2" t="n">
         <v>5.224542126175285</v>
       </c>
       <c r="L2" t="n">
-        <v>29.33168010004412</v>
+        <v>29.77400213642043</v>
       </c>
       <c r="M2" t="n">
-        <v>55.92071004870427</v>
+        <v>56.7704446341448</v>
       </c>
     </row>
     <row r="3">
@@ -612,10 +612,10 @@
         <v>303369.27</v>
       </c>
       <c r="F4" t="n">
-        <v>251.7003107406596</v>
+        <v>254.6468579941883</v>
       </c>
       <c r="G4" t="n">
-        <v>85398933.92443219</v>
+        <v>86396806.08009991</v>
       </c>
       <c r="H4" t="n">
         <v>633260</v>
@@ -624,16 +624,16 @@
         <v>0.7625666666666667</v>
       </c>
       <c r="J4" t="n">
-        <v>134.8560368954808</v>
+        <v>136.4318069672803</v>
       </c>
       <c r="K4" t="n">
         <v>5.202284946236559</v>
       </c>
       <c r="L4" t="n">
-        <v>25.92246258887424</v>
+        <v>26.22536219704341</v>
       </c>
       <c r="M4" t="n">
-        <v>48.3826459607417</v>
+        <v>48.94904078224418</v>
       </c>
     </row>
     <row r="5">
@@ -659,10 +659,10 @@
         <v>90093</v>
       </c>
       <c r="F5" t="n">
-        <v>108.7110506496714</v>
+        <v>109.5570717781737</v>
       </c>
       <c r="G5" t="n">
-        <v>10436345.31444595</v>
+        <v>10516814.6157781</v>
       </c>
       <c r="H5" t="n">
         <v>148241</v>
@@ -671,16 +671,16 @@
         <v>0.7723916666666666</v>
       </c>
       <c r="J5" t="n">
-        <v>70.40120691607551</v>
+        <v>70.94403448289002</v>
       </c>
       <c r="K5" t="n">
         <v>5.75</v>
       </c>
       <c r="L5" t="n">
-        <v>12.24368815931748</v>
+        <v>12.33809295354609</v>
       </c>
       <c r="M5" t="n">
-        <v>18.90626967820372</v>
+        <v>19.05340378750846</v>
       </c>
     </row>
     <row r="6">
@@ -706,10 +706,10 @@
         <v>72809</v>
       </c>
       <c r="F6" t="n">
-        <v>185.8760061596631</v>
+        <v>188.1561850756708</v>
       </c>
       <c r="G6" t="n">
-        <v>15329108.75720448</v>
+        <v>15513484.0253405</v>
       </c>
       <c r="H6" t="n">
         <v>177708</v>
@@ -718,16 +718,16 @@
         <v>0.6250166666666667</v>
       </c>
       <c r="J6" t="n">
-        <v>86.2600938461098</v>
+        <v>87.29761195523272</v>
       </c>
       <c r="K6" t="n">
         <v>5.670888628498197</v>
       </c>
       <c r="L6" t="n">
-        <v>15.21103648776008</v>
+        <v>15.39399160768768</v>
       </c>
       <c r="M6" t="n">
-        <v>32.77722740410933</v>
+        <v>33.17931234447459</v>
       </c>
     </row>
     <row r="7">
@@ -847,10 +847,10 @@
         <v>13055.36</v>
       </c>
       <c r="F9" t="n">
-        <v>149.6391241791543</v>
+        <v>152.0431323330019</v>
       </c>
       <c r="G9" t="n">
-        <v>3778466.406464273</v>
+        <v>3835150.174225295</v>
       </c>
       <c r="H9" t="n">
         <v>49960</v>
@@ -859,16 +859,16 @@
         <v>0.6447111111111111</v>
       </c>
       <c r="J9" t="n">
-        <v>75.62983199488137</v>
+        <v>76.76441501651911</v>
       </c>
       <c r="K9" t="n">
         <v>6.416666666666667</v>
       </c>
       <c r="L9" t="n">
-        <v>11.78646732387762</v>
+        <v>11.96328545711986</v>
       </c>
       <c r="M9" t="n">
-        <v>23.32038298895911</v>
+        <v>23.69503361033796</v>
       </c>
     </row>
     <row r="10">
@@ -894,10 +894,10 @@
         <v>82729.42</v>
       </c>
       <c r="F10" t="n">
-        <v>201.7128065740409</v>
+        <v>203.8725298381634</v>
       </c>
       <c r="G10" t="n">
-        <v>17324188.5798462</v>
+        <v>17507776.58339982</v>
       </c>
       <c r="H10" t="n">
         <v>159720</v>
@@ -906,16 +906,16 @@
         <v>0.8160833333333333</v>
       </c>
       <c r="J10" t="n">
-        <v>108.4659941137378</v>
+        <v>109.6154306498862</v>
       </c>
       <c r="K10" t="n">
         <v>6.333333333333333</v>
       </c>
       <c r="L10" t="n">
-        <v>17.12620959690597</v>
+        <v>17.30769957629782</v>
       </c>
       <c r="M10" t="n">
-        <v>31.84939051169067</v>
+        <v>32.19039944813106</v>
       </c>
     </row>
     <row r="11">
@@ -988,10 +988,10 @@
         <v>264293.59</v>
       </c>
       <c r="F12" t="n">
-        <v>390.965024204828</v>
+        <v>394.2001942322248</v>
       </c>
       <c r="G12" t="n">
-        <v>108305344.7054131</v>
+        <v>109199621.6541033</v>
       </c>
       <c r="H12" t="n">
         <v>459141</v>
@@ -1000,16 +1000,16 @@
         <v>0.8520083333333334</v>
       </c>
       <c r="J12" t="n">
-        <v>235.8868946694221</v>
+        <v>237.8346121433357</v>
       </c>
       <c r="K12" t="n">
         <v>6.488429744387459</v>
       </c>
       <c r="L12" t="n">
-        <v>36.35500482585422</v>
+        <v>36.65518800585989</v>
       </c>
       <c r="M12" t="n">
-        <v>60.25572281845476</v>
+        <v>60.754328822503</v>
       </c>
     </row>
     <row r="13">
@@ -1082,10 +1082,10 @@
         <v>88418.42</v>
       </c>
       <c r="F14" t="n">
-        <v>258.8574364344258</v>
+        <v>261.6614664607744</v>
       </c>
       <c r="G14" t="n">
-        <v>24098261.38468845</v>
+        <v>24357207.70323403</v>
       </c>
       <c r="H14" t="n">
         <v>176880</v>
@@ -1094,16 +1094,16 @@
         <v>0.8058916666666667</v>
       </c>
       <c r="J14" t="n">
-        <v>136.2407360057013</v>
+        <v>137.7047020761761</v>
       </c>
       <c r="K14" t="n">
         <v>6.285445979512827</v>
       </c>
       <c r="L14" t="n">
-        <v>21.67558777050552</v>
+        <v>21.90850140547216</v>
       </c>
       <c r="M14" t="n">
-        <v>41.18362281342674</v>
+        <v>41.6297375418785</v>
       </c>
     </row>
     <row r="15">
@@ -1176,10 +1176,10 @@
         <v>47324.48</v>
       </c>
       <c r="F16" t="n">
-        <v>448.386587461132</v>
+        <v>452.8546878821612</v>
       </c>
       <c r="G16" t="n">
-        <v>23550418.09539641</v>
+        <v>23784104.6119052</v>
       </c>
       <c r="H16" t="n">
         <v>153300</v>
@@ -1188,16 +1188,16 @@
         <v>0.6016833333333333</v>
       </c>
       <c r="J16" t="n">
-        <v>153.623079552488</v>
+        <v>155.1474534370854</v>
       </c>
       <c r="K16" t="n">
         <v>6.928708580206276</v>
       </c>
       <c r="L16" t="n">
-        <v>22.17196433854265</v>
+        <v>22.39197270907106</v>
       </c>
       <c r="M16" t="n">
-        <v>64.71430891783632</v>
+        <v>65.35917662576583</v>
       </c>
     </row>
     <row r="17">
@@ -1223,10 +1223,10 @@
         <v>34858.84</v>
       </c>
       <c r="F17" t="n">
-        <v>408.0426073309466</v>
+        <v>411.5681105642029</v>
       </c>
       <c r="G17" t="n">
-        <v>27646557.3043687</v>
+        <v>27886284.82320945</v>
       </c>
       <c r="H17" t="n">
         <v>149634</v>
@@ -1235,16 +1235,16 @@
         <v>0.7907416666666666</v>
       </c>
       <c r="J17" t="n">
-        <v>184.7611993555522</v>
+        <v>186.3632919203486</v>
       </c>
       <c r="K17" t="n">
         <v>6.87249435815744</v>
       </c>
       <c r="L17" t="n">
-        <v>26.88415438802744</v>
+        <v>27.11727099479407</v>
       </c>
       <c r="M17" t="n">
-        <v>59.37329098664337</v>
+        <v>59.88627841879335</v>
       </c>
     </row>
     <row r="18">
@@ -1270,10 +1270,10 @@
         <v>147502.04</v>
       </c>
       <c r="F18" t="n">
-        <v>306.1560712492274</v>
+        <v>309.4825811310093</v>
       </c>
       <c r="G18" t="n">
-        <v>48722821.35396093</v>
+        <v>49244660.93664289</v>
       </c>
       <c r="H18" t="n">
         <v>338135</v>
@@ -1282,16 +1282,16 @@
         <v>0.7579333333333333</v>
       </c>
       <c r="J18" t="n">
-        <v>144.0928071745336</v>
+        <v>145.6360948634211</v>
       </c>
       <c r="K18" t="n">
         <v>6.990489077264852</v>
       </c>
       <c r="L18" t="n">
-        <v>20.61269327251598</v>
+        <v>20.83346290277071</v>
       </c>
       <c r="M18" t="n">
-        <v>43.79608749335407</v>
+        <v>44.27194974634016</v>
       </c>
     </row>
     <row r="19">
@@ -1317,10 +1317,10 @@
         <v>52529.88</v>
       </c>
       <c r="F19" t="n">
-        <v>502.8746547995295</v>
+        <v>511.8247641200482</v>
       </c>
       <c r="G19" t="n">
-        <v>32665823.11319728</v>
+        <v>33247887.26297089</v>
       </c>
       <c r="H19" t="n">
         <v>153300</v>
@@ -1329,16 +1329,16 @@
         <v>0.876</v>
       </c>
       <c r="J19" t="n">
-        <v>213.0842994990038</v>
+        <v>216.8811954531695</v>
       </c>
       <c r="K19" t="n">
         <v>7.023745519713262</v>
       </c>
       <c r="L19" t="n">
-        <v>30.33770214210477</v>
+        <v>30.87828208531443</v>
       </c>
       <c r="M19" t="n">
-        <v>71.59636598281239</v>
+        <v>72.87063044689339</v>
       </c>
     </row>
     <row r="20">
@@ -1458,10 +1458,10 @@
         <v>320138.94</v>
       </c>
       <c r="F22" t="n">
-        <v>377.9998067401887</v>
+        <v>382.5674025459423</v>
       </c>
       <c r="G22" t="n">
-        <v>149555732.0788243</v>
+        <v>151358304.6767375</v>
       </c>
       <c r="H22" t="n">
         <v>934591</v>
@@ -1470,16 +1470,16 @@
         <v>0.8227833333333333</v>
       </c>
       <c r="J22" t="n">
-        <v>160.022653844114</v>
+        <v>161.9513826655055</v>
       </c>
       <c r="K22" t="n">
         <v>7.416666666666667</v>
       </c>
       <c r="L22" t="n">
-        <v>21.57608815875694</v>
+        <v>21.83614148298951</v>
       </c>
       <c r="M22" t="n">
-        <v>50.9662660773288</v>
+        <v>51.58212169158772</v>
       </c>
     </row>
     <row r="23">
@@ -1505,10 +1505,10 @@
         <v>40838.15</v>
       </c>
       <c r="F23" t="n">
-        <v>317.146799467298</v>
+        <v>319.4937778679435</v>
       </c>
       <c r="G23" t="n">
-        <v>22800273.31730439</v>
+        <v>22962171.73611701</v>
       </c>
       <c r="H23" t="n">
         <v>204992</v>
@@ -1517,16 +1517,16 @@
         <v>0.5416249999999999</v>
       </c>
       <c r="J23" t="n">
-        <v>111.2251859453266</v>
+        <v>112.0149651504303</v>
       </c>
       <c r="K23" t="n">
         <v>7.273521505376344</v>
       </c>
       <c r="L23" t="n">
-        <v>15.29179309679811</v>
+        <v>15.40037587950109</v>
       </c>
       <c r="M23" t="n">
-        <v>43.60292318279031</v>
+        <v>43.92559747459114</v>
       </c>
     </row>
     <row r="24">
@@ -1552,10 +1552,10 @@
         <v>26382.56</v>
       </c>
       <c r="F24" t="n">
-        <v>214.1592643831008</v>
+        <v>215.5050416447036</v>
       </c>
       <c r="G24" t="n">
-        <v>6131662.448662853</v>
+        <v>6168599.512652317</v>
       </c>
       <c r="H24" t="n">
         <v>39003</v>
@@ -1564,16 +1564,16 @@
         <v>0.8929416666666666</v>
       </c>
       <c r="J24" t="n">
-        <v>157.2100209897406</v>
+        <v>158.1570523460328</v>
       </c>
       <c r="K24" t="n">
         <v>7.333333333333333</v>
       </c>
       <c r="L24" t="n">
-        <v>21.43773013496463</v>
+        <v>21.56687077445902</v>
       </c>
       <c r="M24" t="n">
-        <v>29.20353605224102</v>
+        <v>29.38705113336867</v>
       </c>
     </row>
     <row r="25">
@@ -1599,10 +1599,10 @@
         <v>145830.13</v>
       </c>
       <c r="F25" t="n">
-        <v>404.2435043783969</v>
+        <v>411.9436297660876</v>
       </c>
       <c r="G25" t="n">
-        <v>90849205.98219676</v>
+        <v>92571022.36643706</v>
       </c>
       <c r="H25" t="n">
         <v>453692</v>
@@ -1611,16 +1611,16 @@
         <v>0.8358416666666667</v>
       </c>
       <c r="J25" t="n">
-        <v>200.2442317303297</v>
+        <v>204.0393534962862</v>
       </c>
       <c r="K25" t="n">
         <v>7.381209519484064</v>
       </c>
       <c r="L25" t="n">
-        <v>27.12891853316833</v>
+        <v>27.64307840844873</v>
       </c>
       <c r="M25" t="n">
-        <v>54.76656682232386</v>
+        <v>55.80977327342983</v>
       </c>
     </row>
     <row r="26">
@@ -1646,10 +1646,10 @@
         <v>51285.37</v>
       </c>
       <c r="F26" t="n">
-        <v>374.7265187202827</v>
+        <v>385.7288799402649</v>
       </c>
       <c r="G26" t="n">
-        <v>34530739.92515773</v>
+        <v>35545606.28596731</v>
       </c>
       <c r="H26" t="n">
         <v>160160</v>
@@ -1658,16 +1658,16 @@
         <v>0.854675</v>
       </c>
       <c r="J26" t="n">
-        <v>215.6015230092266</v>
+        <v>221.9381011861096</v>
       </c>
       <c r="K26" t="n">
         <v>7.75</v>
       </c>
       <c r="L26" t="n">
-        <v>27.81955135602923</v>
+        <v>28.63717434659479</v>
       </c>
       <c r="M26" t="n">
-        <v>48.35180886713326</v>
+        <v>49.77146837938902</v>
       </c>
     </row>
     <row r="27">
@@ -1693,10 +1693,10 @@
         <v>160789.07</v>
       </c>
       <c r="F27" t="n">
-        <v>482.0453417031387</v>
+        <v>490.9815975211757</v>
       </c>
       <c r="G27" t="n">
-        <v>114165313.2529743</v>
+        <v>116266901.3094148</v>
       </c>
       <c r="H27" t="n">
         <v>470592</v>
@@ -1705,16 +1705,16 @@
         <v>0.83955</v>
       </c>
       <c r="J27" t="n">
-        <v>242.5993498677715</v>
+        <v>247.0651887609964</v>
       </c>
       <c r="K27" t="n">
         <v>7.850933734691807</v>
       </c>
       <c r="L27" t="n">
-        <v>30.90070023082355</v>
+        <v>31.46952924456126</v>
       </c>
       <c r="M27" t="n">
-        <v>61.39974657703078</v>
+        <v>62.53798772388307</v>
       </c>
     </row>
     <row r="28">
@@ -1787,10 +1787,10 @@
         <v>395689.56</v>
       </c>
       <c r="F29" t="n">
-        <v>404.0062959816952</v>
+        <v>409.0416064941321</v>
       </c>
       <c r="G29" t="n">
-        <v>196718709.7061751</v>
+        <v>199164655.1709391</v>
       </c>
       <c r="H29" t="n">
         <v>1224940</v>
@@ -1799,16 +1799,16 @@
         <v>0.7956500000000001</v>
       </c>
       <c r="J29" t="n">
-        <v>160.5945676573344</v>
+        <v>162.591355634512</v>
       </c>
       <c r="K29" t="n">
         <v>7.769698708073977</v>
       </c>
       <c r="L29" t="n">
-        <v>20.66934300688527</v>
+        <v>20.92633984192375</v>
       </c>
       <c r="M29" t="n">
-        <v>51.99767856659193</v>
+        <v>52.64574880736</v>
       </c>
     </row>
     <row r="30">
@@ -1834,10 +1834,10 @@
         <v>166182.76</v>
       </c>
       <c r="F30" t="n">
-        <v>238.596500386941</v>
+        <v>240.9175228078685</v>
       </c>
       <c r="G30" t="n">
-        <v>42607340.67733214</v>
+        <v>43019836.26603248</v>
       </c>
       <c r="H30" t="n">
         <v>322439</v>
@@ -1846,16 +1846,16 @@
         <v>0.844825</v>
       </c>
       <c r="J30" t="n">
-        <v>132.1407791158394</v>
+        <v>133.4200771805907</v>
       </c>
       <c r="K30" t="n">
         <v>8.337409085675555</v>
       </c>
       <c r="L30" t="n">
-        <v>15.84914183266712</v>
+        <v>16.00258255407172</v>
       </c>
       <c r="M30" t="n">
-        <v>28.61758346449283</v>
+        <v>28.89596999885579</v>
       </c>
     </row>
     <row r="31">
@@ -1928,10 +1928,10 @@
         <v>68348.87</v>
       </c>
       <c r="F32" t="n">
-        <v>368.4760040924052</v>
+        <v>371.2418378297348</v>
       </c>
       <c r="G32" t="n">
-        <v>54186850.22538488</v>
+        <v>54566501.55957337</v>
       </c>
       <c r="H32" t="n">
         <v>356610</v>
@@ -1940,16 +1940,16 @@
         <v>0.567725</v>
       </c>
       <c r="J32" t="n">
-        <v>151.9498898667589</v>
+        <v>153.0145020037951</v>
       </c>
       <c r="K32" t="n">
         <v>8.629232279859185</v>
       </c>
       <c r="L32" t="n">
-        <v>17.60873794316711</v>
+        <v>17.73211069551741</v>
       </c>
       <c r="M32" t="n">
-        <v>42.70090225203882</v>
+        <v>43.02142134894449</v>
       </c>
     </row>
     <row r="33">
@@ -1975,10 +1975,10 @@
         <v>35929.88</v>
       </c>
       <c r="F33" t="n">
-        <v>269.29228739463</v>
+        <v>271.4578161450656</v>
       </c>
       <c r="G33" t="n">
-        <v>7358265.253040846</v>
+        <v>7405305.943708388</v>
       </c>
       <c r="H33" t="n">
         <v>104751.4137931034</v>
@@ -1987,16 +1987,16 @@
         <v>0.4490166666666667</v>
       </c>
       <c r="J33" t="n">
-        <v>70.24502091756297</v>
+        <v>70.69409066243966</v>
       </c>
       <c r="K33" t="n">
         <v>9.464135304659498</v>
       </c>
       <c r="L33" t="n">
-        <v>7.422233374345259</v>
+        <v>7.469683007134808</v>
       </c>
       <c r="M33" t="n">
-        <v>28.45397690606228</v>
+        <v>28.68279112740688</v>
       </c>
     </row>
     <row r="34">
@@ -2069,10 +2069,10 @@
         <v>21558.62</v>
       </c>
       <c r="F35" t="n">
-        <v>327.6118297652475</v>
+        <v>330.6426781546463</v>
       </c>
       <c r="G35" t="n">
-        <v>8721588.334591584</v>
+        <v>8798651.309854053</v>
       </c>
       <c r="H35" t="n">
         <v>72240</v>
@@ -2081,16 +2081,16 @@
         <v>0.544875</v>
       </c>
       <c r="J35" t="n">
-        <v>120.7307355286764</v>
+        <v>121.7974987521325</v>
       </c>
       <c r="K35" t="n">
         <v>8.94513888888889</v>
       </c>
       <c r="L35" t="n">
-        <v>13.49679832010667</v>
+        <v>13.61605451463945</v>
       </c>
       <c r="M35" t="n">
-        <v>36.62456601676549</v>
+        <v>36.96339232533892</v>
       </c>
     </row>
     <row r="36">

</xml_diff>